<commit_message>
integrate new stick 2 data from dartmouth
</commit_message>
<xml_diff>
--- a/data/sampling/dartmouth_cfa/cfa_metadata.xlsx
+++ b/data/sampling/dartmouth_cfa/cfa_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Liam/Desktop/UW/ECM/2024_structure/github/data/sampling/dartmouth_cfa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851FC212-76D3-DC44-8EF9-9598EF6077D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68D158A-494A-3D40-A242-CA1D5EDC554E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="760" windowWidth="29180" windowHeight="18880" xr2:uid="{45584F9A-9778-5B4B-A064-AEADAAAF97A5}"/>
   </bookViews>
@@ -480,7 +480,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
got behind on commits. Big update brings everything up to speed
</commit_message>
<xml_diff>
--- a/data/sampling/dartmouth_cfa/cfa_metadata.xlsx
+++ b/data/sampling/dartmouth_cfa/cfa_metadata.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Liam/Desktop/UW/ECM/2024_structure/github/data/sampling/dartmouth_cfa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68D158A-494A-3D40-A242-CA1D5EDC554E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9660C50D-4978-0545-AB88-991331ED38CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="760" windowWidth="29180" windowHeight="18880" xr2:uid="{45584F9A-9778-5B4B-A064-AEADAAAF97A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -912,10 +912,11 @@
         <v>15</v>
       </c>
       <c r="D14" s="1">
-        <v>0</v>
+        <f>9+16+0</f>
+        <v>25</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>156.77000000000001</v>
       </c>
       <c r="F14">
         <v>25</v>
@@ -944,10 +945,11 @@
         <v>16</v>
       </c>
       <c r="D15" s="1">
-        <v>0</v>
+        <f>9+16+4</f>
+        <v>29</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>156.77000000000001</v>
       </c>
       <c r="F15">
         <v>29</v>
@@ -976,10 +978,11 @@
         <v>17</v>
       </c>
       <c r="D16" s="1">
-        <v>0</v>
+        <f>9+16+10</f>
+        <v>35</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>156.77000000000001</v>
       </c>
       <c r="F16">
         <v>35</v>

</xml_diff>